<commit_message>
ADD save/load cinfigure programm,updata method's save_sostav_gaz in data_model
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -436,37 +436,37 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pin_2_0</t>
+          <t>Pin_3_0</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Pin_2_2</t>
+          <t>Pin_3_2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Pin_2_4</t>
+          <t>Pin_3_4</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Pin_2_6</t>
+          <t>Pin_3_6</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Pin_2_8</t>
+          <t>Pin_3_8</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Pin_3_0</t>
+          <t>Pin_4_0</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Pin_3_2</t>
+          <t>Pin_4_2</t>
         </is>
       </c>
     </row>
@@ -475,25 +475,25 @@
         <v>0.6</v>
       </c>
       <c r="B2" t="n">
-        <v>9333.719859776651</v>
+        <v>27289.41365097705</v>
       </c>
       <c r="C2" t="n">
-        <v>10203.54219118979</v>
+        <v>28997.03757680443</v>
       </c>
       <c r="D2" t="n">
-        <v>11070.19800195315</v>
+        <v>30699.11894048838</v>
       </c>
       <c r="E2" t="n">
-        <v>11933.77162257655</v>
+        <v>32395.85801142112</v>
       </c>
       <c r="F2" t="n">
-        <v>12794.35015788826</v>
+        <v>34087.45887438462</v>
       </c>
       <c r="G2" t="n">
-        <v>13652.02326498353</v>
+        <v>35774.12905413556</v>
       </c>
       <c r="H2" t="n">
-        <v>14506.8829418758</v>
+        <v>37456.07915945948</v>
       </c>
     </row>
     <row r="3">
@@ -501,25 +501,25 @@
         <v>0.8</v>
       </c>
       <c r="B3" t="n">
-        <v>9352.453423409786</v>
+        <v>27343.41092200421</v>
       </c>
       <c r="C3" t="n">
-        <v>10223.8824665669</v>
+        <v>29053.96309513143</v>
       </c>
       <c r="D3" t="n">
-        <v>11092.11143018891</v>
+        <v>30758.90060446428</v>
       </c>
       <c r="E3" t="n">
-        <v>11957.22430269087</v>
+        <v>32458.42349011225</v>
       </c>
       <c r="F3" t="n">
-        <v>12819.30790308839</v>
+        <v>34152.73569285308</v>
       </c>
       <c r="G3" t="n">
-        <v>13678.45165513043</v>
+        <v>35842.0446720012</v>
       </c>
       <c r="H3" t="n">
-        <v>14534.74737229862</v>
+        <v>37526.5610430948</v>
       </c>
     </row>
     <row r="4">
@@ -527,25 +527,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>9272.738776784594</v>
+        <v>27397.72999821576</v>
       </c>
       <c r="C4" t="n">
-        <v>10244.34487105289</v>
+        <v>29111.2251950953</v>
       </c>
       <c r="D4" t="n">
-        <v>11114.15550847628</v>
+        <v>30819.03288010401</v>
       </c>
       <c r="E4" t="n">
-        <v>11980.81579867541</v>
+        <v>32521.35286902505</v>
       </c>
       <c r="F4" t="n">
-        <v>12844.41227451241</v>
+        <v>34218.388964855</v>
       </c>
       <c r="G4" t="n">
-        <v>13705.03412683362</v>
+        <v>35910.34856884402</v>
       </c>
       <c r="H4" t="n">
-        <v>14562.77298575765</v>
+        <v>37597.44231171037</v>
       </c>
     </row>
     <row r="5">
@@ -553,25 +553,25 @@
         <v>1.2</v>
       </c>
       <c r="B5" t="n">
-        <v>8777.326498513889</v>
+        <v>27452.37408877807</v>
       </c>
       <c r="C5" t="n">
-        <v>9942.117393182705</v>
+        <v>29168.82720664944</v>
       </c>
       <c r="D5" t="n">
-        <v>11037.98764122716</v>
+        <v>30879.51920801507</v>
       </c>
       <c r="E5" t="n">
-        <v>12004.54748536933</v>
+        <v>32584.64968948758</v>
       </c>
       <c r="F5" t="n">
-        <v>12869.66471351646</v>
+        <v>34284.42232272403</v>
       </c>
       <c r="G5" t="n">
-        <v>13731.77218313442</v>
+        <v>35979.04445852413</v>
       </c>
       <c r="H5" t="n">
-        <v>14590.96134222041</v>
+        <v>37668.72675146379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>